<commit_message>
Added animation on cards  +  excel
</commit_message>
<xml_diff>
--- a/Docs/Sprint 2/B65_S2_Suivi_CarvalhoYohann.xlsx
+++ b/Docs/Sprint 2/B65_S2_Suivi_CarvalhoYohann.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yohann\Documents\GitHub\Final-Project\Docs\Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DCBF11-C567-4E7E-BFB6-009BA19B33E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBE2078-BA77-4B47-9974-B5C8BB837ED9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="494" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="494" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 - Planification" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="115">
   <si>
     <t>B65 - Projet Synthèse  |  Sprint 1  |  Planification</t>
   </si>
@@ -514,6 +514,21 @@
   <si>
     <t>À finir en prioritaire sprint 3 le plus tot possible</t>
   </si>
+  <si>
+    <t>Annulé</t>
+  </si>
+  <si>
+    <t>n'existe pas car pas besoin</t>
+  </si>
+  <si>
+    <t>Pas de rest</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Annulé (Optionnelle)</t>
+  </si>
 </sst>
 </file>
 
@@ -522,7 +537,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -726,12 +741,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1581,60 +1590,6 @@
   </cellStyles>
   <dxfs count="89">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDCDEE0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFE00000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE5E5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B400"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD1FFD1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEDEEEF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF40000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF1F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00C000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5FFE5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1782,6 +1737,60 @@
       <font>
         <strike/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCDEE0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFE00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE5E5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B400"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD1FFD1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDEEEF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFF40000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF1F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00C000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE5FFE5"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2928,7 +2937,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3347,7 +3356,7 @@
                   <c:v>39.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>21.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9841,7 +9850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:W56"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -11263,8 +11272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:Z57"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13196,32 +13205,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>AND($D28="Sprint 3",$H28&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="19" priority="5">
       <formula>AND($D28&lt;&gt;"Sprint 3",$H28&lt;1,NOT(ISBLANK($H28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28">
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="18" priority="6">
       <formula>LEN($B28)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>AND($D29="Sprint 3",$H29&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>AND($D29&lt;&gt;"Sprint 3",$H29&lt;1,NOT(ISBLANK($H29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>LEN($B29)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" xWindow="1092" yWindow="513" count="6">
+  <dataValidations xWindow="1092" yWindow="513" count="6">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Nom de tâche trop long" error="Le nom de votre tâche doit être court. _x000a_Un maximum de 72 caractères est mis à votre disposition._x000a_Pour plus de détail, veuillez faire l'ajout de commentaires." promptTitle="Nom de la tâche" prompt="_x000a_Veuillez saisir le nom de la tâche._x000a__x000a_Lorsque pertinent, n'oubliez pas d'ajouter une description de votre tâche sous forme de commentaire." sqref="C9:C43" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>0</formula1>
       <formula2>72</formula2>
@@ -13252,8 +13261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:Z57"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13318,7 +13327,7 @@
       <c r="H5" s="35"/>
       <c r="I5" s="64" t="str">
         <f>IF(M45=0,CONCATENATE("Ce sprint totalise ", W15, " de travail réalisé. ",W16),CONCATENATE("Attention, il reste ",M46," à remplir!"))</f>
-        <v>Attention, il reste 38 champs à remplir!</v>
+        <v>Ce sprint totalise 21 heures et 45 minutes de travail réalisé. 10 tâches n'ont pas été terminé!</v>
       </c>
     </row>
     <row r="6" spans="2:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -13415,7 +13424,7 @@
       </c>
       <c r="V9" s="9">
         <f>SUM(G9:G43)</f>
-        <v>0</v>
+        <v>0.90625000000000022</v>
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.25">
@@ -13463,15 +13472,15 @@
       </c>
       <c r="S10" s="61">
         <f t="array" ref="S10">SUM(($D$9:$D$43=$R10)*$G$9:$G$43)</f>
-        <v>0</v>
+        <v>0.71875</v>
       </c>
       <c r="T10" s="62">
         <f t="shared" ref="T10:T11" si="4">S10*24*60</f>
-        <v>0</v>
+        <v>1035</v>
       </c>
       <c r="V10" s="10">
         <f>V9</f>
-        <v>0</v>
+        <v>0.90625000000000022</v>
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.25">
@@ -13519,15 +13528,15 @@
       </c>
       <c r="S11" s="61">
         <f t="array" ref="S11">SUM(($D$9:$D$43=$R11)*$G$9:$G$43)</f>
-        <v>0</v>
+        <v>0.18750000000000031</v>
       </c>
       <c r="T11" s="62">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>270.00000000000045</v>
       </c>
       <c r="V11" s="63">
         <f>DAY(V9)*24+HOUR(V9)</f>
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
@@ -13574,7 +13583,7 @@
       <c r="R12" s="8"/>
       <c r="V12" s="4">
         <f>MINUTE(V9)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
@@ -13623,11 +13632,11 @@
       </c>
       <c r="V13" s="63">
         <f>V11</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="W13" s="4" t="str">
         <f>V13 &amp; " " &amp; U13 &amp; IF(V13 &gt; 1, "s", "")</f>
-        <v>0 heure</v>
+        <v>21 heures</v>
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
@@ -13676,11 +13685,11 @@
       </c>
       <c r="V14" s="4">
         <f>V12</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="W14" s="4" t="str">
         <f>V14 &amp; " " &amp; U14 &amp; IF(V14 &gt; 1, "s", "")</f>
-        <v>0 minute</v>
+        <v>45 minutes</v>
       </c>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
@@ -13726,11 +13735,11 @@
       <c r="R15" s="8"/>
       <c r="W15" s="4" t="str">
         <f>IF(V13&gt;0,IF(V14&gt;0,W13&amp;" et "&amp;W14,W13),W14)</f>
-        <v>0 minute</v>
+        <v>21 heures et 45 minutes</v>
       </c>
       <c r="Y15" s="4" t="str">
         <f>V13&amp;"h"&amp;TEXT(V14,"00")</f>
-        <v>0h00</v>
+        <v>21h45</v>
       </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
@@ -13776,11 +13785,11 @@
       <c r="R16" s="8"/>
       <c r="V16" s="4">
         <f>P44</f>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="W16" s="4" t="str">
         <f>IF(V16=0,"",IF(V16=1,"Une tâche n'a pas été terminée!",CONCATENATE(V16," tâches n'ont pas été terminé!")))</f>
-        <v>19 tâches n'ont pas été terminé!</v>
+        <v>10 tâches n'ont pas été terminé!</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
@@ -14056,16 +14065,22 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H23)&lt;&gt;0,'Sprint 2 - Bilan'!$H23,IF(LEN('Sprint 2 - Bilan'!$F23)=0,"",'Sprint 2 - Bilan'!$F23))</f>
         <v/>
       </c>
-      <c r="G23" s="109"/>
-      <c r="H23" s="110"/>
-      <c r="I23" s="111"/>
+      <c r="G23" s="109">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="H23" s="110">
+        <v>1</v>
+      </c>
+      <c r="I23" s="111" t="s">
+        <v>113</v>
+      </c>
       <c r="M23" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N23" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O23" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14073,7 +14088,7 @@
       </c>
       <c r="P23" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R23" s="8"/>
     </row>
@@ -14098,16 +14113,22 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H24)&lt;&gt;0,'Sprint 2 - Bilan'!$H24,IF(LEN('Sprint 2 - Bilan'!$F24)=0,"",'Sprint 2 - Bilan'!$F24))</f>
         <v/>
       </c>
-      <c r="G24" s="106"/>
-      <c r="H24" s="107"/>
-      <c r="I24" s="108"/>
+      <c r="G24" s="106">
+        <v>0</v>
+      </c>
+      <c r="H24" s="107">
+        <v>0</v>
+      </c>
+      <c r="I24" s="108" t="s">
+        <v>114</v>
+      </c>
       <c r="M24" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N24" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O24" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14182,16 +14203,20 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H26)&lt;&gt;0,'Sprint 2 - Bilan'!$H26,IF(LEN('Sprint 2 - Bilan'!$F26)=0,"",'Sprint 2 - Bilan'!$F26))</f>
         <v>0.5</v>
       </c>
-      <c r="G26" s="106"/>
-      <c r="H26" s="107"/>
+      <c r="G26" s="106">
+        <v>0.1875</v>
+      </c>
+      <c r="H26" s="107">
+        <v>1</v>
+      </c>
       <c r="I26" s="108"/>
       <c r="M26" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N26" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O26" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14199,7 +14224,7 @@
       </c>
       <c r="P26" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R26" s="8"/>
     </row>
@@ -14224,16 +14249,20 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H27)&lt;&gt;0,'Sprint 2 - Bilan'!$H27,IF(LEN('Sprint 2 - Bilan'!$F27)=0,"",'Sprint 2 - Bilan'!$F27))</f>
         <v>0</v>
       </c>
-      <c r="G27" s="112"/>
-      <c r="H27" s="110"/>
+      <c r="G27" s="112">
+        <v>0.125</v>
+      </c>
+      <c r="H27" s="110">
+        <v>1</v>
+      </c>
       <c r="I27" s="111"/>
       <c r="M27" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N27" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O27" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14241,7 +14270,7 @@
       </c>
       <c r="P27" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R27" s="8"/>
     </row>
@@ -14266,16 +14295,22 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H28)&lt;&gt;0,'Sprint 2 - Bilan'!$H28,IF(LEN('Sprint 2 - Bilan'!$F28)=0,"",'Sprint 2 - Bilan'!$F28))</f>
         <v>0</v>
       </c>
-      <c r="G28" s="106"/>
-      <c r="H28" s="107"/>
-      <c r="I28" s="108"/>
+      <c r="G28" s="106">
+        <v>0</v>
+      </c>
+      <c r="H28" s="107">
+        <v>0</v>
+      </c>
+      <c r="I28" s="108" t="s">
+        <v>111</v>
+      </c>
       <c r="M28" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N28" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O28" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14308,16 +14343,20 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H29)&lt;&gt;0,'Sprint 2 - Bilan'!$H29,IF(LEN('Sprint 2 - Bilan'!$F29)=0,"",'Sprint 2 - Bilan'!$F29))</f>
         <v>0.7</v>
       </c>
-      <c r="G29" s="109"/>
-      <c r="H29" s="110"/>
+      <c r="G29" s="109">
+        <v>7.2916666666666699E-2</v>
+      </c>
+      <c r="H29" s="110">
+        <v>1</v>
+      </c>
       <c r="I29" s="111"/>
       <c r="M29" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N29" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O29" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14325,7 +14364,7 @@
       </c>
       <c r="P29" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R29" s="8"/>
     </row>
@@ -14350,16 +14389,22 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H30)&lt;&gt;0,'Sprint 2 - Bilan'!$H30,IF(LEN('Sprint 2 - Bilan'!$F30)=0,"",'Sprint 2 - Bilan'!$F30))</f>
         <v/>
       </c>
-      <c r="G30" s="106"/>
-      <c r="H30" s="107"/>
-      <c r="I30" s="108"/>
+      <c r="G30" s="106">
+        <v>0</v>
+      </c>
+      <c r="H30" s="107">
+        <v>0</v>
+      </c>
+      <c r="I30" s="108" t="s">
+        <v>114</v>
+      </c>
       <c r="M30" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N30" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O30" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14392,16 +14437,20 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H31)&lt;&gt;0,'Sprint 2 - Bilan'!$H31,IF(LEN('Sprint 2 - Bilan'!$F31)=0,"",'Sprint 2 - Bilan'!$F31))</f>
         <v>0</v>
       </c>
-      <c r="G31" s="112"/>
-      <c r="H31" s="110"/>
+      <c r="G31" s="112">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="H31" s="110">
+        <v>1</v>
+      </c>
       <c r="I31" s="111"/>
       <c r="M31" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N31" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O31" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14409,7 +14458,7 @@
       </c>
       <c r="P31" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R31" s="8"/>
     </row>
@@ -14434,16 +14483,22 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H32)&lt;&gt;0,'Sprint 2 - Bilan'!$H32,IF(LEN('Sprint 2 - Bilan'!$F32)=0,"",'Sprint 2 - Bilan'!$F32))</f>
         <v>0.7</v>
       </c>
-      <c r="G32" s="106"/>
-      <c r="H32" s="107"/>
-      <c r="I32" s="108"/>
+      <c r="G32" s="106">
+        <v>6.25E-2</v>
+      </c>
+      <c r="H32" s="107">
+        <v>1</v>
+      </c>
+      <c r="I32" s="108" t="s">
+        <v>112</v>
+      </c>
       <c r="M32" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N32" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O32" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14451,7 +14506,7 @@
       </c>
       <c r="P32" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R32" s="8"/>
     </row>
@@ -14476,16 +14531,22 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H33)&lt;&gt;0,'Sprint 2 - Bilan'!$H33,IF(LEN('Sprint 2 - Bilan'!$F33)=0,"",'Sprint 2 - Bilan'!$F33))</f>
         <v/>
       </c>
-      <c r="G33" s="112"/>
-      <c r="H33" s="110"/>
-      <c r="I33" s="111"/>
+      <c r="G33" s="112">
+        <v>0</v>
+      </c>
+      <c r="H33" s="110">
+        <v>0</v>
+      </c>
+      <c r="I33" s="111" t="s">
+        <v>114</v>
+      </c>
       <c r="M33" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N33" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O33" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14518,16 +14579,22 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H34)&lt;&gt;0,'Sprint 2 - Bilan'!$H34,IF(LEN('Sprint 2 - Bilan'!$F34)=0,"",'Sprint 2 - Bilan'!$F34))</f>
         <v/>
       </c>
-      <c r="G34" s="106"/>
-      <c r="H34" s="107"/>
-      <c r="I34" s="108"/>
+      <c r="G34" s="106">
+        <v>0</v>
+      </c>
+      <c r="H34" s="107">
+        <v>0</v>
+      </c>
+      <c r="I34" s="108" t="s">
+        <v>114</v>
+      </c>
       <c r="M34" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N34" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O34" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14560,16 +14627,20 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H35)&lt;&gt;0,'Sprint 2 - Bilan'!$H35,IF(LEN('Sprint 2 - Bilan'!$F35)=0,"",'Sprint 2 - Bilan'!$F35))</f>
         <v/>
       </c>
-      <c r="G35" s="109"/>
-      <c r="H35" s="110"/>
+      <c r="G35" s="109">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="H35" s="110">
+        <v>1</v>
+      </c>
       <c r="I35" s="111"/>
       <c r="M35" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N35" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O35" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14577,7 +14648,7 @@
       </c>
       <c r="P35" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R35" s="8"/>
     </row>
@@ -14602,16 +14673,20 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H36)&lt;&gt;0,'Sprint 2 - Bilan'!$H36,IF(LEN('Sprint 2 - Bilan'!$F36)=0,"",'Sprint 2 - Bilan'!$F36))</f>
         <v>0</v>
       </c>
-      <c r="G36" s="106"/>
-      <c r="H36" s="107"/>
+      <c r="G36" s="106">
+        <v>0.114583333333333</v>
+      </c>
+      <c r="H36" s="107">
+        <v>1</v>
+      </c>
       <c r="I36" s="108"/>
       <c r="M36" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N36" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O36" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14619,7 +14694,7 @@
       </c>
       <c r="P36" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R36" s="8"/>
     </row>
@@ -14644,16 +14719,20 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H37)&lt;&gt;0,'Sprint 2 - Bilan'!$H37,IF(LEN('Sprint 2 - Bilan'!$F37)=0,"",'Sprint 2 - Bilan'!$F37))</f>
         <v>0</v>
       </c>
-      <c r="G37" s="112"/>
-      <c r="H37" s="110"/>
+      <c r="G37" s="112">
+        <v>5.2083333333333301E-2</v>
+      </c>
+      <c r="H37" s="110">
+        <v>1</v>
+      </c>
       <c r="I37" s="111"/>
       <c r="M37" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N37" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O37" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14661,7 +14740,7 @@
       </c>
       <c r="P37" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R37" s="8"/>
     </row>
@@ -14686,16 +14765,22 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H38)&lt;&gt;0,'Sprint 2 - Bilan'!$H38,IF(LEN('Sprint 2 - Bilan'!$F38)=0,"",'Sprint 2 - Bilan'!$F38))</f>
         <v/>
       </c>
-      <c r="G38" s="106"/>
-      <c r="H38" s="107"/>
-      <c r="I38" s="108"/>
+      <c r="G38" s="106">
+        <v>0</v>
+      </c>
+      <c r="H38" s="107">
+        <v>0</v>
+      </c>
+      <c r="I38" s="108" t="s">
+        <v>110</v>
+      </c>
       <c r="M38" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N38" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O38" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14728,16 +14813,22 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H39)&lt;&gt;0,'Sprint 2 - Bilan'!$H39,IF(LEN('Sprint 2 - Bilan'!$F39)=0,"",'Sprint 2 - Bilan'!$F39))</f>
         <v/>
       </c>
-      <c r="G39" s="112"/>
-      <c r="H39" s="110"/>
-      <c r="I39" s="111"/>
+      <c r="G39" s="112">
+        <v>0</v>
+      </c>
+      <c r="H39" s="110">
+        <v>0</v>
+      </c>
+      <c r="I39" s="111" t="s">
+        <v>110</v>
+      </c>
       <c r="M39" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N39" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O39" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14770,16 +14861,22 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H40)&lt;&gt;0,'Sprint 2 - Bilan'!$H40,IF(LEN('Sprint 2 - Bilan'!$F40)=0,"",'Sprint 2 - Bilan'!$F40))</f>
         <v/>
       </c>
-      <c r="G40" s="106"/>
-      <c r="H40" s="107"/>
-      <c r="I40" s="108"/>
+      <c r="G40" s="106">
+        <v>0</v>
+      </c>
+      <c r="H40" s="107">
+        <v>0</v>
+      </c>
+      <c r="I40" s="108" t="s">
+        <v>114</v>
+      </c>
       <c r="M40" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N40" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O40" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14812,16 +14909,22 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H41)&lt;&gt;0,'Sprint 2 - Bilan'!$H41,IF(LEN('Sprint 2 - Bilan'!$F41)=0,"",'Sprint 2 - Bilan'!$F41))</f>
         <v/>
       </c>
-      <c r="G41" s="109"/>
-      <c r="H41" s="110"/>
-      <c r="I41" s="111"/>
+      <c r="G41" s="109">
+        <v>0</v>
+      </c>
+      <c r="H41" s="110">
+        <v>0</v>
+      </c>
+      <c r="I41" s="111" t="s">
+        <v>110</v>
+      </c>
       <c r="M41" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N41" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O41" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14854,16 +14957,22 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H42)&lt;&gt;0,'Sprint 2 - Bilan'!$H42,IF(LEN('Sprint 2 - Bilan'!$F42)=0,"",'Sprint 2 - Bilan'!$F42))</f>
         <v/>
       </c>
-      <c r="G42" s="106"/>
-      <c r="H42" s="107"/>
-      <c r="I42" s="108"/>
+      <c r="G42" s="106">
+        <v>0</v>
+      </c>
+      <c r="H42" s="107">
+        <v>0</v>
+      </c>
+      <c r="I42" s="108" t="s">
+        <v>110</v>
+      </c>
       <c r="M42" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N42" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O42" s="3" t="b">
         <f t="shared" si="2"/>
@@ -14920,11 +15029,11 @@
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M44" s="3">
         <f>COUNTIF(M9:M43,TRUE)</f>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="N44" s="3">
         <f t="shared" ref="N44:O44" si="5">COUNTIF(N9:N43,TRUE)</f>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" si="5"/>
@@ -14932,21 +15041,21 @@
       </c>
       <c r="P44" s="3">
         <f>COUNTIF(P9:P43,FALSE)</f>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="R44" s="8"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M45" s="3">
         <f>SUM(M44:O44)</f>
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="R45" s="8"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M46" s="3" t="str">
         <f>IF(M45=0, "aucun champ", IF(M45=1, "1 champ", M45 &amp; " champs"))</f>
-        <v>38 champs</v>
+        <v>aucun champ</v>
       </c>
       <c r="R46" s="8"/>
     </row>
@@ -14997,50 +15106,50 @@
     <mergeCell ref="I7:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="B9:F43">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>OR($F9=100%,$H9=100%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>AND($D9&lt;&gt;"Sprint 3",$F9=100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:I9 G11:I11 G13:I13 G15:I15 G17:I17 G19:I19 G21:I21 G23:I23 G25:I25 G27:I27 G29:I29 G31:I31 G33:I33 G35:I35 G37:I37 G39:I39 G41:I41 G43:I43">
-    <cfRule type="expression" dxfId="18" priority="11">
+    <cfRule type="expression" dxfId="12" priority="11">
       <formula>IF(ISBLANK($H9),IF(ISBLANK($F9),TRUE,$F9&lt;100%),$H9&lt;100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:I10 G12:I12 G14:I14 G16:I16 G18:I18 G20:I20 G22:I22 G24:I24 G26:I26 G28:I28 G30:I30 G32:I32 G34:I34 G36:I36 G38:I38 G40:I40 G42:I42">
-    <cfRule type="expression" dxfId="17" priority="8">
+    <cfRule type="expression" dxfId="11" priority="8">
       <formula>IF(ISBLANK($H10),IF(ISBLANK($F10),TRUE,$F10&lt;100%),$H10&lt;100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I43">
-    <cfRule type="expression" dxfId="16" priority="6">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>$O9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:G43">
-    <cfRule type="expression" dxfId="15" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>$M9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H43">
-    <cfRule type="expression" dxfId="14" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>$N9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="13" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$M$45&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:I9 B11:I11 B13:I13 B15:I15 B17:I17 B19:I19 B21:I21 B23:I23 B25:I25 B27:I27 B29:I29 B31:I31 B33:I33 B35:I35 B37:I37 B39:I39 B41:I41 B43:I43">
-    <cfRule type="expression" dxfId="12" priority="12">
+    <cfRule type="expression" dxfId="6" priority="12">
       <formula>LEN($B9)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:I10 B12:I12 B14:I14 B16:I16 B18:I18 B20:I20 B22:I22 B24:I24 B26:I26 B28:I28 B30:I30 B32:I32 B34:I34 B36:I36 B38:I38 B40:I40 B42:I42">
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>LEN($B10)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15069,7 +15178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:Y23"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A13" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="AY27" sqref="AY27"/>
     </sheetView>
   </sheetViews>
@@ -15280,11 +15389,11 @@
       </c>
       <c r="E10" s="91" t="str">
         <f t="shared" si="0"/>
-        <v>0h00</v>
+        <v>21h45</v>
       </c>
       <c r="F10" s="95" t="str">
         <f t="shared" si="0"/>
-        <v>50h30</v>
+        <v>72h15</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -15298,11 +15407,11 @@
       </c>
       <c r="N10" s="1">
         <f>'Sprint 3 - Bilan'!V9</f>
-        <v>0</v>
+        <v>0.90625000000000022</v>
       </c>
       <c r="O10" s="1">
         <f>SUM(L10:N10)</f>
-        <v>2.104166666666667</v>
+        <v>3.010416666666667</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>47</v>
@@ -15317,7 +15426,7 @@
       </c>
       <c r="S10" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>21.75</v>
       </c>
       <c r="U10" s="2" t="s">
         <v>48</v>
@@ -15348,11 +15457,11 @@
       </c>
       <c r="E11" s="100">
         <f>N11</f>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F11" s="101">
         <f>O11</f>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -15366,11 +15475,11 @@
       </c>
       <c r="N11" s="1">
         <f>'Sprint 3 - Bilan'!V16</f>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="O11" s="1">
         <f>N11</f>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
@@ -15503,7 +15612,7 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="ZTHIqTmr8cTliRMGAcUcmM0mjbf6CIJ0mHH1g8KtGLF4lRA/UYuFPwpT4A16q2cQqIx/6PesESjQGKIAV9ov5g==" saltValue="9FKXXuq3MsinQZgjNrQSTw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <conditionalFormatting sqref="F5:J5">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15826,22 +15935,22 @@
     <mergeCell ref="C35:G35"/>
   </mergeCells>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="9" priority="69">
+    <cfRule type="expression" dxfId="3" priority="69">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16023,18 +16132,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16057,18 +16166,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16325D0D-63D9-490D-8587-E384C7BFA0C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20DD170F-C51C-4776-BE86-DE3613560936}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16325D0D-63D9-490D-8587-E384C7BFA0C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>